<commit_message>
Please merge code in main ,Please do not delete branch  __12_08_2022
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/MarketoData.xlsx
+++ b/src/test/resources/TestData/MarketoData.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20388"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{121CBA23-E200-4F73-A841-AA01F5462557}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9900" windowHeight="3600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14180" windowHeight="3570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Interesting Moment</t>
   </si>
@@ -77,15 +76,60 @@
     <t>19</t>
   </si>
   <si>
-    <t>8</t>
+    <t>Snippets</t>
+  </si>
+  <si>
+    <t>Account Name</t>
+  </si>
+  <si>
+    <t>send_box</t>
+  </si>
+  <si>
+    <t>Event Programs</t>
+  </si>
+  <si>
+    <t>Nurture campaigns</t>
+  </si>
+  <si>
+    <t>Segment Data</t>
+  </si>
+  <si>
+    <t>Library</t>
+  </si>
+  <si>
+    <t>Integration Data</t>
+  </si>
+  <si>
+    <t>Interesting Moment_subscription</t>
+  </si>
+  <si>
+    <t>Web Personalize</t>
+  </si>
+  <si>
+    <t>Images and Files</t>
+  </si>
+  <si>
+    <t>Models</t>
+  </si>
+  <si>
+    <t>Leads</t>
+  </si>
+  <si>
+    <t>All Batch Campaigns</t>
+  </si>
+  <si>
+    <t>Tokens</t>
+  </si>
+  <si>
+    <t>Target Account Management</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +141,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF131313"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -143,10 +194,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,19 +479,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -446,31 +499,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="n">
-        <v>21.0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="n">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="n">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -478,7 +531,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -486,7 +539,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -494,7 +547,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -502,7 +555,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -510,7 +563,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -518,20 +571,140 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TestNG Optimaize with One login
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/MarketoData.xlsx
+++ b/src/test/resources/TestData/MarketoData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20388"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20389"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{121CBA23-E200-4F73-A841-AA01F5462557}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60582AC7-6B9C-4385-BD28-66D6A89944CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9900" windowHeight="3600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="33">
   <si>
     <t>Interesting Moment</t>
   </si>
@@ -65,27 +64,15 @@
     <t>Tags</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
     <t>All Triggered Campaigns</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
     <t>8</t>
   </si>
   <si>
     <t>Batch Campaigns - Repeating Schedule</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>All Batch Campaigns</t>
   </si>
   <si>
@@ -113,9 +100,6 @@
     <t>Models</t>
   </si>
   <si>
-    <t>were</t>
-  </si>
-  <si>
     <t>Segmentations</t>
   </si>
   <si>
@@ -125,19 +109,16 @@
     <t>Interesting Moment Subscription</t>
   </si>
   <si>
-    <t>False</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
+    <t>Account Name</t>
+  </si>
+  <si>
     <t>True</t>
   </si>
   <si>
-    <t>Account Name</t>
-  </si>
-  <si>
-    <t>sandboxcopy clone07</t>
+    <t>sandboxcopy_23may_07 Marketo</t>
   </si>
 </sst>
 </file>
@@ -489,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,7 +487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -514,7 +495,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -522,7 +503,7 @@
         <v>6.0</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -530,7 +511,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -538,128 +519,140 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>25</v>
-      </c>
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>29</v>
       </c>
       <c r="B17" t="n">
         <v>0.0</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B18" t="n">
         <v>2.0</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
       <c r="B19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
       <c r="B20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
       <c r="B21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Event And Nurture Code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/MarketoData.xlsx
+++ b/src/test/resources/TestData/MarketoData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20389"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB7909E-B2D1-45D7-8CF5-B17C06739914}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032691E5-D3B5-4434-9B58-50555D7179EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9900" windowHeight="3600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16260" windowHeight="3600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3679" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="43">
   <si>
     <t>Interesting Moment</t>
   </si>
@@ -73,21 +73,12 @@
     <t>All Batch Campaigns</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>Images and Files</t>
   </si>
   <si>
     <t>Leads</t>
   </si>
   <si>
-    <t>241</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -115,52 +106,49 @@
     <t>sandboxcopy_23may_07 Marketo</t>
   </si>
   <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Models</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Campaign Data</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>WP_DEMO</t>
+  </si>
+  <si>
+    <t>Asset Data</t>
+  </si>
+  <si>
+    <t>Database Data</t>
+  </si>
+  <si>
+    <t>Program Data</t>
+  </si>
+  <si>
+    <t>Total WorkSpace</t>
+  </si>
+  <si>
+    <t>Event Programs</t>
+  </si>
+  <si>
     <t>Nurture campaigns</t>
   </si>
   <si>
-    <t>Event Programs</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>Models</t>
-  </si>
-  <si>
-    <t>WorkSpace Name</t>
-  </si>
-  <si>
-    <t>Default</t>
-  </si>
-  <si>
-    <t>Automation</t>
-  </si>
-  <si>
-    <t>World</t>
-  </si>
-  <si>
-    <t>Campaign Data</t>
-  </si>
-  <si>
-    <t>Total</t>
+    <t>5</t>
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>WP_DEMO</t>
-  </si>
-  <si>
-    <t>Asset Data</t>
-  </si>
-  <si>
-    <t>Database Data</t>
-  </si>
-  <si>
-    <t>Program Data</t>
-  </si>
-  <si>
-    <t>Total WorkSpace</t>
   </si>
 </sst>
 </file>
@@ -510,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,7 +509,7 @@
     <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -531,19 +519,19 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
@@ -551,10 +539,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C3" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D3" t="n">
         <v>0.0</v>
@@ -599,7 +587,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" t="n">
         <v>1.0</v>
@@ -616,7 +604,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B7" t="n">
         <v>0.0</v>
@@ -633,19 +621,19 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
@@ -659,10 +647,10 @@
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10">
@@ -676,10 +664,10 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
@@ -690,13 +678,13 @@
         <v>0.0</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
@@ -713,7 +701,7 @@
         <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13">
@@ -724,13 +712,13 @@
         <v>10.0</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14">
@@ -744,32 +732,32 @@
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B16" t="n">
         <v>2.0</v>
@@ -786,41 +774,41 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B17" t="n">
-        <v>482.0</v>
+        <v>723.0</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0</v>
+        <v>241.0</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0</v>
+        <v>241.0</v>
       </c>
       <c r="E17" t="n">
-        <v>0.0</v>
+        <v>241.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B19" t="n">
         <v>0.0</v>
@@ -835,39 +823,39 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20">
       <c r="A20" t="s">
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21">
       <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
         <v>25</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -893,9 +881,25 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B27" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" t="n">
         <v>3.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
final commit on report Date: 2/16/2022
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/MarketoData.xlsx
+++ b/src/test/resources/TestData/MarketoData.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20389"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032691E5-D3B5-4434-9B58-50555D7179EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16260" windowHeight="3600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16260" windowHeight="3600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="47">
   <si>
     <t>Interesting Moment</t>
   </si>
@@ -43,109 +42,121 @@
     <t>1</t>
   </si>
   <si>
+    <t>All Campaigns</t>
+  </si>
+  <si>
+    <t>Active Campaigns</t>
+  </si>
+  <si>
+    <t>Active Triggered Campaigns</t>
+  </si>
+  <si>
+    <t>All Triggered Campaigns</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Batch Campaigns - Repeating Schedule</t>
+  </si>
+  <si>
+    <t>All Batch Campaigns</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Integration</t>
+  </si>
+  <si>
+    <t>Interesting Moment Subscription</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Account Name</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>sandboxcopy_23may_07 Marketo</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Campaign Data</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>WP_DEMO</t>
+  </si>
+  <si>
+    <t>Total WorkSpace</t>
+  </si>
+  <si>
+    <t>Event Programs</t>
+  </si>
+  <si>
+    <t>Nurture campaigns</t>
+  </si>
+  <si>
+    <t>Library</t>
+  </si>
+  <si>
+    <t>Web Personalize</t>
+  </si>
+  <si>
+    <t>Target Account Management</t>
+  </si>
+  <si>
+    <t>Predictive Content</t>
+  </si>
+  <si>
     <t>Forms</t>
   </si>
   <si>
     <t>Landing Pages</t>
   </si>
   <si>
-    <t>All Campaigns</t>
-  </si>
-  <si>
-    <t>Active Campaigns</t>
-  </si>
-  <si>
-    <t>Active Triggered Campaigns</t>
+    <t>Images and Files</t>
+  </si>
+  <si>
+    <t>Snippets</t>
+  </si>
+  <si>
+    <t>Asset Data</t>
   </si>
   <si>
     <t>Tags</t>
   </si>
   <si>
-    <t>All Triggered Campaigns</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>Batch Campaigns - Repeating Schedule</t>
-  </si>
-  <si>
-    <t>All Batch Campaigns</t>
-  </si>
-  <si>
-    <t>Images and Files</t>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Segmentations</t>
   </si>
   <si>
     <t>Leads</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>Snippets</t>
-  </si>
-  <si>
-    <t>Segmentations</t>
-  </si>
-  <si>
-    <t>Integration</t>
-  </si>
-  <si>
-    <t>Interesting Moment Subscription</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Account Name</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>sandboxcopy_23may_07 Marketo</t>
-  </si>
-  <si>
-    <t>9</t>
+    <t>Database Data</t>
   </si>
   <si>
     <t>Models</t>
   </si>
   <si>
-    <t>Default</t>
-  </si>
-  <si>
-    <t>Automation</t>
-  </si>
-  <si>
-    <t>Campaign Data</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>WP_DEMO</t>
-  </si>
-  <si>
-    <t>Asset Data</t>
-  </si>
-  <si>
-    <t>Database Data</t>
-  </si>
-  <si>
     <t>Program Data</t>
-  </si>
-  <si>
-    <t>Total WorkSpace</t>
-  </si>
-  <si>
-    <t>Event Programs</t>
-  </si>
-  <si>
-    <t>Nurture campaigns</t>
-  </si>
-  <si>
-    <t>5</t>
   </si>
   <si>
     <t/>
@@ -154,7 +165,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -497,11 +508,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD32"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,19 +530,19 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3">
@@ -553,7 +564,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="B4" t="n">
         <v>2.0</v>
@@ -570,7 +581,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="B5" t="n">
         <v>3.0</v>
@@ -587,7 +598,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B6" t="n">
         <v>1.0</v>
@@ -604,7 +615,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B7" t="n">
         <v>0.0</v>
@@ -620,144 +631,81 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
       <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
       <c r="B9" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
+        <v>0.0</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
       <c r="B10" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
+        <v>0.0</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
       <c r="B11" t="n">
         <v>0.0</v>
       </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
-      </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
       <c r="B12" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
+        <v>0.0</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
       <c r="B13" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="C13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" t="s">
-        <v>6</v>
+        <v>0.0</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
       <c r="B14" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" t="s">
-        <v>19</v>
+        <v>0.0</v>
       </c>
       <c r="E14" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B16" t="n">
         <v>2.0</v>
@@ -774,7 +722,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="B17" t="n">
         <v>723.0</v>
@@ -786,32 +734,26 @@
         <v>241.0</v>
       </c>
       <c r="E17" t="n">
-        <v>241.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E18" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" t="n">
-        <v>0.0</v>
+        <v>44</v>
       </c>
       <c r="C19" t="n">
         <v>0.0</v>
@@ -819,40 +761,40 @@
       <c r="D19" t="n">
         <v>0.0</v>
       </c>
-      <c r="E19" t="n">
-        <v>0.0</v>
+      <c r="E19" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24">
@@ -881,15 +823,15 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B27" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B28" t="n">
         <v>2.0</v>
@@ -897,10 +839,42 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B29" t="n">
         <v>3.0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest Specific Workspace and Add On Element
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/MarketoData.xlsx
+++ b/src/test/resources/TestData/MarketoData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7453" uniqueCount="73">
   <si>
     <t>Interesting Moment</t>
   </si>
@@ -149,6 +149,96 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Target Account Management</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>Predictive Content</t>
+  </si>
+  <si>
+    <t>Web Personalization</t>
+  </si>
+  <si>
+    <t>1-50</t>
+  </si>
+  <si>
+    <t>1349</t>
+  </si>
+  <si>
+    <t>148</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>984</t>
+  </si>
+  <si>
+    <t>3002</t>
+  </si>
+  <si>
+    <t>217</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>.Customer Support New Hire Workspace</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>ACT-SS</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Alicia's Ally</t>
+  </si>
+  <si>
+    <t>C.COEL</t>
+  </si>
+  <si>
+    <t>2689</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>Pradyumna Sahoo</t>
+  </si>
+  <si>
+    <t>2688</t>
   </si>
 </sst>
 </file>
@@ -498,7 +588,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A31" sqref="A31:XFD32"/>
@@ -525,13 +615,13 @@
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3">
@@ -539,16 +629,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>2.0</v>
+        <v>7.0</v>
       </c>
       <c r="C3" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4">
@@ -556,16 +646,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="D4" t="n">
         <v>2.0</v>
       </c>
-      <c r="C4" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.0</v>
+      <c r="E4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5">
@@ -573,16 +663,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>3.0</v>
+        <v>71.0</v>
       </c>
       <c r="C5" t="n">
-        <v>3.0</v>
+        <v>64.0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="6">
@@ -590,16 +680,16 @@
         <v>17</v>
       </c>
       <c r="B6" t="n">
+        <v>582.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>581.0</v>
+      </c>
+      <c r="D6" t="n">
         <v>1.0</v>
       </c>
-      <c r="C6" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.0</v>
+      <c r="E6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="7">
@@ -607,16 +697,16 @@
         <v>20</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="8">
@@ -627,13 +717,13 @@
         <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9">
@@ -641,16 +731,16 @@
         <v>13</v>
       </c>
       <c r="B9" t="n">
-        <v>8.0</v>
+        <v>40.0</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
+        <v>58</v>
+      </c>
+      <c r="F9" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10">
@@ -658,16 +748,16 @@
         <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
       </c>
-      <c r="E10" t="s">
-        <v>19</v>
+      <c r="F10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="11">
@@ -683,8 +773,8 @@
       <c r="D11" t="s">
         <v>19</v>
       </c>
-      <c r="E11" t="s">
-        <v>19</v>
+      <c r="F11" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="12">
@@ -692,16 +782,16 @@
         <v>16</v>
       </c>
       <c r="B12" t="n">
-        <v>2.0</v>
+        <v>84.0</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13">
@@ -709,16 +799,16 @@
         <v>9</v>
       </c>
       <c r="B13" t="n">
-        <v>10.0</v>
+        <v>128.0</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14">
@@ -726,16 +816,16 @@
         <v>10</v>
       </c>
       <c r="B14" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
         <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15">
@@ -746,10 +836,10 @@
         <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="E15" t="s">
         <v>34</v>
@@ -760,10 +850,10 @@
         <v>21</v>
       </c>
       <c r="B16" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="C16" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="D16" t="n">
         <v>0.0</v>
@@ -777,13 +867,13 @@
         <v>18</v>
       </c>
       <c r="B17" t="n">
-        <v>723.0</v>
+        <v>198.0</v>
       </c>
       <c r="C17" t="n">
-        <v>241.0</v>
+        <v>0.0</v>
       </c>
       <c r="D17" t="n">
-        <v>241.0</v>
+        <v>0.0</v>
       </c>
       <c r="E17" t="n">
         <v>241.0</v>
@@ -797,10 +887,10 @@
         <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="E18" t="s">
         <v>34</v>
@@ -811,10 +901,10 @@
         <v>29</v>
       </c>
       <c r="B19" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D19" t="n">
         <v>0.0</v>
@@ -828,7 +918,7 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21">
@@ -836,7 +926,7 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22">
@@ -852,7 +942,7 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24">
@@ -884,7 +974,7 @@
         <v>38</v>
       </c>
       <c r="B27" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -901,6 +991,30 @@
       </c>
       <c r="B29" t="n">
         <v>3.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>